<commit_message>
Update requirements.txt with gigachat and yandex-cloud-ml-sdk dependencies and update config.xlsx
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projects\LLM_trust_games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD0A1B6-E020-4E33-9B27-70AAD0894F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA97ED4-97A5-456B-AB96-064D1150E9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9975" yWindow="1050" windowWidth="15660" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,7 +595,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,13 +637,13 @@
         <v>52</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -660,13 +660,13 @@
         <v>53</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,13 +683,13 @@
         <v>67</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -706,13 +706,13 @@
         <v>54</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,13 +729,13 @@
         <v>55</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>59</v>
@@ -755,13 +755,13 @@
         <v>55</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>60</v>
@@ -781,13 +781,13 @@
         <v>55</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
         <v>61</v>
@@ -807,13 +807,13 @@
         <v>55</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>62</v>
@@ -833,13 +833,13 @@
         <v>55</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>63</v>
@@ -859,13 +859,13 @@
         <v>55</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>64</v>
@@ -885,13 +885,13 @@
         <v>55</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>65</v>
@@ -911,13 +911,13 @@
         <v>55</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>66</v>
@@ -937,13 +937,13 @@
         <v>56</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
         <v>59</v>
@@ -963,13 +963,13 @@
         <v>56</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
         <v>60</v>
@@ -989,13 +989,13 @@
         <v>56</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
@@ -1015,13 +1015,13 @@
         <v>56</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
         <v>62</v>
@@ -1041,13 +1041,13 @@
         <v>56</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
         <v>63</v>
@@ -1067,13 +1067,13 @@
         <v>56</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H19" t="s">
         <v>64</v>
@@ -1093,13 +1093,13 @@
         <v>56</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H20" t="s">
         <v>65</v>
@@ -1119,13 +1119,13 @@
         <v>56</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
         <v>66</v>
@@ -1145,13 +1145,13 @@
         <v>57</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G22">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
         <v>59</v>
@@ -1171,13 +1171,13 @@
         <v>57</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H23" t="s">
         <v>60</v>
@@ -1197,13 +1197,13 @@
         <v>57</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H24" t="s">
         <v>61</v>
@@ -1223,13 +1223,13 @@
         <v>57</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>62</v>
@@ -1249,13 +1249,13 @@
         <v>57</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G26">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H26" t="s">
         <v>63</v>
@@ -1275,13 +1275,13 @@
         <v>57</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G27">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H27" t="s">
         <v>64</v>
@@ -1301,13 +1301,13 @@
         <v>57</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H28" t="s">
         <v>65</v>
@@ -1327,13 +1327,13 @@
         <v>57</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H29" t="s">
         <v>66</v>
@@ -1353,13 +1353,13 @@
         <v>58</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G30">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H30" t="s">
         <v>59</v>
@@ -1379,13 +1379,13 @@
         <v>58</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G31">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H31" t="s">
         <v>60</v>
@@ -1405,13 +1405,13 @@
         <v>58</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
         <v>61</v>
@@ -1431,13 +1431,13 @@
         <v>58</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G33">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
         <v>62</v>
@@ -1457,13 +1457,13 @@
         <v>58</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G34">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
         <v>63</v>
@@ -1483,13 +1483,13 @@
         <v>58</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G35">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H35" t="s">
         <v>64</v>
@@ -1509,13 +1509,13 @@
         <v>58</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
         <v>65</v>
@@ -1535,13 +1535,13 @@
         <v>58</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G37">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
         <v>66</v>

</xml_diff>